<commit_message>
fix 0.7999999999999 => 0.8 issue
</commit_message>
<xml_diff>
--- a/tests/samples/test_formula.xlsx
+++ b/tests/samples/test_formula.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,21 +19,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -61,7 +61,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,12 +345,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <f>0.1+0.1</f>
         <v>0.2</v>
@@ -372,10 +372,10 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <f>0.6+0.3</f>
-        <v>0.89999999999999991</v>
+        <f>0.1+0.7</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="B2">
         <f>0.2+0.2</f>

</xml_diff>

<commit_message>
add check_if_skip for skipping validation when this check is true
</commit_message>
<xml_diff>
--- a/tests/samples/test_formula.xlsx
+++ b/tests/samples/test_formula.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,21 +19,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -61,7 +61,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,12 +345,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1">
         <f>0.1+0.1</f>
         <v>0.2</v>
@@ -372,10 +372,10 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <f>0.6+0.3</f>
-        <v>0.89999999999999991</v>
+        <f>0.1+0.7</f>
+        <v>0.79999999999999993</v>
       </c>
       <c r="B2">
         <f>0.2+0.2</f>

</xml_diff>